<commit_message>
trying to figure out master program corruption
</commit_message>
<xml_diff>
--- a/JustinHours.xlsx
+++ b/JustinHours.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juxin\source\BassMidi\Midi-Bass-Guitar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEDAB4C-7329-4AB2-89BD-DA120F32B6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4030C19F-B0D2-473E-A3AD-29036B3036A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="W1" sheetId="1" r:id="rId1"/>
+    <sheet name="W2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -67,11 +68,20 @@
   <si>
     <t>I2C troubleshooting</t>
   </si>
+  <si>
+    <t>Justin Week One Hours</t>
+  </si>
+  <si>
+    <t>Justin Week Two Hours</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -131,6 +141,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -413,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +450,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -545,10 +572,12 @@
       <c r="C8" s="4">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="4">
+        <v>0.625</v>
+      </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>13.25</v>
+        <v>1.7499999999999991</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>9</v>
@@ -558,215 +587,269 @@
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="3">
+        <v>45757</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>0.99999999999999911</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="3">
+        <v>45757</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>1.2499999999999982</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="3">
+        <v>45758</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="3">
+        <v>45758</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="3">
+        <v>45759</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.625</v>
+      </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>1.7499999999999991</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="3">
+        <v>45759</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>0.99999999999999911</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="3">
+        <v>45760</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>1.2499999999999982</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="3">
+        <v>45760</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="15">
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:I2"/>
@@ -778,18 +861,273 @@
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F13:I13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D217EFE-31D6-4852-88BC-72D89609389D}">
+  <dimension ref="B2:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>45761</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E4" s="10">
+        <f>ABS((D4-C4)*24)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>45761</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" ref="E5:E16" si="0">ABS((D5-C5)*24)</f>
+        <v>1.8333333333333321</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>45762</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7499999999999996</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>45762</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>13.25</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>45763</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>45763</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fret slave program v1 + updated hours
</commit_message>
<xml_diff>
--- a/JustinHours.xlsx
+++ b/JustinHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juxin\source\BassMidi\Midi-Bass-Guitar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4030C19F-B0D2-473E-A3AD-29036B3036A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EFA22D-3164-4DC0-9ADE-1220AD6AD851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Justin Week Two Hours</t>
+  </si>
+  <si>
+    <t>Finalizing Fret Slave</t>
+  </si>
+  <si>
+    <t>Investigationg MIDI over IR</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -122,11 +131,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,12 +158,33 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -153,9 +192,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I25"/>
+  <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,16 +489,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -474,12 +513,12 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
@@ -495,12 +534,12 @@
         <f>ABS((D4-C4)*24)</f>
         <v>0.99999999999999911</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -513,15 +552,15 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E24" si="0">ABS((D5-C5)*24)</f>
+        <f t="shared" ref="E5:E16" si="0">ABS((D5-C5)*24)</f>
         <v>1.2499999999999982</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -537,12 +576,12 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -558,12 +597,12 @@
         <f t="shared" si="0"/>
         <v>1.9999999999999996</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -579,12 +618,12 @@
         <f t="shared" si="0"/>
         <v>1.7499999999999991</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="F8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
@@ -600,12 +639,12 @@
         <f t="shared" si="0"/>
         <v>0.99999999999999911</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="F9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
@@ -621,12 +660,12 @@
         <f t="shared" si="0"/>
         <v>1.2499999999999982</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="F10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
@@ -642,12 +681,12 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="F11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
@@ -663,12 +702,12 @@
         <f t="shared" si="0"/>
         <v>1.9999999999999996</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
@@ -684,12 +723,12 @@
         <f t="shared" si="0"/>
         <v>1.7499999999999991</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="F13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -705,12 +744,12 @@
         <f t="shared" si="0"/>
         <v>0.99999999999999911</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="F14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -726,12 +765,12 @@
         <f t="shared" si="0"/>
         <v>1.2499999999999982</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="F15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
@@ -747,120 +786,90 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="F16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUM(E4:E16)</f>
+        <v>18.749999999999993</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -871,22 +880,22 @@
   <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -901,12 +910,12 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
@@ -918,16 +927,16 @@
       <c r="D4" s="4">
         <v>0.4861111111111111</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <f>ABS((D4-C4)*24)</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="F4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -939,16 +948,16 @@
       <c r="D5" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <f t="shared" ref="E5:E16" si="0">ABS((D5-C5)*24)</f>
         <v>1.8333333333333321</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="F5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -964,12 +973,12 @@
         <f t="shared" si="0"/>
         <v>2.7499999999999996</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="F6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -978,73 +987,95 @@
       <c r="C7" s="4">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>13.25</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="D7" s="4">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>1.416666666666667</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>45763</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="C8" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>45763</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="3">
+        <v>45764</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+        <v>9.25</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>45764</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -1054,10 +1085,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
@@ -1067,67 +1098,60 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="17">
+        <f>SUM(E4:E13)</f>
+        <v>23.583333333333329</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
+  <mergeCells count="12">
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="F11:I11"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F13:I13"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hours + added IR schematics + updated fret code header
</commit_message>
<xml_diff>
--- a/JustinHours.xlsx
+++ b/JustinHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juxin\source\BassMidi\Midi-Bass-Guitar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06C2A79-3E32-4CB6-8840-8864BB0EB459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7BE1B-0023-4763-8B23-7B5256224682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Write up for MIDI over IR</t>
+  </si>
+  <si>
+    <t>Write up for fret slave</t>
+  </si>
+  <si>
+    <t>Justin Week Three Hours</t>
+  </si>
+  <si>
+    <t>Justin Week Four Hours</t>
   </si>
 </sst>
 </file>
@@ -870,7 +882,7 @@
   <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D13"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,14 +1188,14 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1440,11 +1452,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F12:I12"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="F3:I3"/>
@@ -1452,6 +1459,11 @@
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1462,14 +1474,14 @@
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1545,11 +1557,15 @@
       <c r="B6" s="3">
         <v>45776</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C6" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>13</v>
@@ -1562,11 +1578,15 @@
       <c r="B7" s="3">
         <v>45776</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4">
+        <v>0.53125</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.61111111111111116</v>
+      </c>
       <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9166666666666679</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>13</v>
@@ -1579,13 +1599,19 @@
       <c r="B8" s="3">
         <v>45777</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.4861111111111111</v>
+      </c>
       <c r="E8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="13"/>
+        <v>2.4166666666666661</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
@@ -1594,13 +1620,19 @@
       <c r="B9" s="3">
         <v>45777</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="13"/>
+        <v>3.4999999999999982</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -1609,13 +1641,19 @@
       <c r="B10" s="3">
         <v>45778</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="13"/>
+      <c r="C10" s="4">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333326</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -1624,13 +1662,19 @@
       <c r="B11" s="3">
         <v>45778</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.625</v>
+      </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="13"/>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
@@ -1673,7 +1717,7 @@
       </c>
       <c r="E14" s="12">
         <f>SUM(E4:E13)</f>
-        <v>3.8333333333333357</v>
+        <v>18.416666666666668</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1682,11 +1726,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F12:I12"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="F3:I3"/>
@@ -1694,6 +1733,11 @@
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>